<commit_message>
Finishing report. Revision is required.
</commit_message>
<xml_diff>
--- a/output/kruskal_wallis_test/anova_Q15_Escola.xlsx
+++ b/output/kruskal_wallis_test/anova_Q15_Escola.xlsx
@@ -365,13 +365,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>96.9428124765355</v>
+        <v>93.86620999825</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0000000000000000000000713588985257395</v>
+        <v>0.000000000000000000000337588280678456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>